<commit_message>
Updates for 2024 data
</commit_message>
<xml_diff>
--- a/resources/prais2021.xlsx
+++ b/resources/prais2021.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Projects\PRAiS2\xlsx-to-edn\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C659FB9-4ACE-4F34-84FA-BEFC168155AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD61E2CC-2117-4301-A416-02E1DB4B1AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="3675" windowWidth="21922" windowHeight="12330" xr2:uid="{39E2FD11-D2A6-4789-9E25-05694701A385}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="35805" windowHeight="19635" xr2:uid="{39E2FD11-D2A6-4789-9E25-05694701A385}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +20,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -453,9 +447,9 @@
       <selection sqref="A1:J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -519,7 +513,7 @@
         <v>0.99304347826086536</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -551,7 +545,7 @@
         <v>0.99555555555555708</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -583,7 +577,7 @@
         <v>0.99243379571248225</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -615,7 +609,7 @@
         <v>0.99210526315789771</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -647,7 +641,7 @@
         <v>0.9937629937629916</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -679,7 +673,7 @@
         <v>0.98837209302326023</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -711,7 +705,7 @@
         <v>0.99098196392786042</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -743,7 +737,7 @@
         <v>0.99732262382864911</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -775,7 +769,7 @@
         <v>0.99050332383665329</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -807,7 +801,7 @@
         <v>0.98728813559322048</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -841,5 +835,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>